<commit_message>
Reordenament dels directoris. Ara el codi s'enmmagatzema en /scripts i genera les figures corresponents al directori corresponent en /plots. Tot i que cal revisar les dades de l'Excel, en principi el diagrama de Clapeyron està pràcticament complet, cal veure com s'ajusta a l'informe en LateX
</commit_message>
<xml_diff>
--- a/graphs/practica_IIIb/datos_isotermas.xlsx
+++ b/graphs/practica_IIIb/datos_isotermas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel\UAB\TERCER\LAB Termo\pIIIb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel\UAB\TERCER\LAB Termo\Repositori\graphs\practica_IIIb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DA14BD-C675-4EE2-8172-51CB8F3B432B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B54DC-82F6-4A5B-B4E2-1296559A04AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-870" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Semana 2" sheetId="1" r:id="rId1"/>
@@ -309,11 +309,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -336,17 +342,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -389,7 +389,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>25.3ºC</c:v>
+            <c:v>10</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -415,156 +415,150 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Semana 2'!$D$5:$D$27</c:f>
+              <c:f>'Datos Semana 2'!$L$37:$L$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>9.5</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>10.5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>11.5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>13.5</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>14.5</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>15.5</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>16.5</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>18</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.6</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>35</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Datos Semana 2'!$U$5:$U$27</c:f>
+              <c:f>'Datos Semana 2'!$AA$37:$AA$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>38</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38</c:v>
+                  <c:v>36.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.800000000000004</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.4</c:v>
+                  <c:v>35.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.800000000000004</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.4</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.1</c:v>
+                  <c:v>32.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.799999999999997</c:v>
+                  <c:v>32.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.1</c:v>
+                  <c:v>31.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32.4</c:v>
+                  <c:v>29.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>31.200000000000003</c:v>
+                  <c:v>28.049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30.099999999999998</c:v>
+                  <c:v>27.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.599999999999998</c:v>
+                  <c:v>23.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24</c:v>
+                  <c:v>20.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.200000000000003</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.399999999999999</c:v>
+                  <c:v>13.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.8000000000000007</c:v>
+                  <c:v>10.199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.35</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.15</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.1000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.25</c:v>
+                  <c:v>3.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -572,7 +566,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ECAC-42E5-B1F5-9FCCF299A255}"/>
+              <c16:uniqueId val="{00000000-AD05-486C-8381-EB62D2948BC5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -580,7 +574,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>44,7ºC</c:v>
+            <c:v>15+'Datos Semana 2'!$D$37:$D$56</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -606,549 +600,6 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Datos Semana 2'!$H$5:$H$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>26.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>29.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>32.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>37.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>37.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>42</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$X$5:$X$27</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>38.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>37.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>34.4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>33.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>29.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>21.599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18.75</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>11.4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.75</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8.4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ECAC-42E5-B1F5-9FCCF299A255}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>20.2ºC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$L$5:$L$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>31</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$AA$5:$AA$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37.800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>37.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36.800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35.1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>31.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>30.400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>28.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25.8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>21.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12.9</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.6000000000000005</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.6499999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-ECAC-42E5-B1F5-9FCCF299A255}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>40ºC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$P$5:$P$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>33.5</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>33.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>38.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$AD$5:$AD$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39.9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>36.800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37.700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>36.300000000000004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>35.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>33.6</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>24.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20.099999999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>13.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-ECAC-42E5-B1F5-9FCCF299A255}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>15,7ºC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
               <c:f>'Datos Semana 2'!$D$37:$D$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -1288,369 +739,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-ECAC-42E5-B1F5-9FCCF299A255}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>35ºC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$H$37:$H$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>22.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>24.5</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>30.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>35.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$X$37:$X$56</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
-                <c:pt idx="0">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>39.9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>39.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39.1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>38.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>37.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37.700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>37.199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>36.300000000000004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>34.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>32.800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>31.499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>29.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>27.5</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>12.200000000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.1000000000000005</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-ECAC-42E5-B1F5-9FCCF299A255}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>10,9ºC</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$L$37:$L$58</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$AA$37:$AA$58</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>36.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35.699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>34.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>31.900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29.7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>28.049999999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>27.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>23.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>20.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13.600000000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>10.199999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-ECAC-42E5-B1F5-9FCCF299A255}"/>
+              <c16:uniqueId val="{00000001-AD05-486C-8381-EB62D2948BC5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1662,11 +751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1152812400"/>
-        <c:axId val="1152814320"/>
+        <c:axId val="2139939551"/>
+        <c:axId val="2139932831"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1152812400"/>
+        <c:axId val="2139939551"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,12 +812,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1152814320"/>
+        <c:crossAx val="2139932831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1152814320"/>
+        <c:axId val="2139932831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1785,529 +874,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1152812400"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:dLblPos val="ctr"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-2F12-4C45-B065-AA333EA48A19}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$L$37:$L$58</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>17.5</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>18.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Semana 2'!$M$37:$M$58</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.2000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.65</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2F12-4C45-B065-AA333EA48A19}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="1501661392"/>
-        <c:axId val="1501658032"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1501661392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1501658032"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="1501658032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1501661392"/>
+        <c:crossAx val="2139939551"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2364,46 +931,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2959,543 +1486,27 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>95758</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>3260</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68852</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>832493</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>3260</xdr:rowOff>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>96338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Gráfico 5">
+        <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B046087C-630E-9A56-0B91-111D518A9A04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{925D366A-CB05-F14F-DFAB-A4D341D1E19D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3508,42 +1519,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>978626</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>161677</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>324064</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>111603</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Gráfico 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41D08484-D4F0-86BC-47AE-AB065AF23B16}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3841,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AE80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView tabSelected="1" topLeftCell="I9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE30" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3886,126 +1861,126 @@
       </c>
     </row>
     <row r="2" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="L2" s="23" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="23" t="s">
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="P2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="U2" s="13" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="U2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="13"/>
-      <c r="X2" s="13" t="s">
+      <c r="V2" s="24"/>
+      <c r="X2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="AA2" s="13" t="s">
+      <c r="Y2" s="24"/>
+      <c r="AA2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="13"/>
-      <c r="AD2" s="13" t="s">
+      <c r="AB2" s="24"/>
+      <c r="AD2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AE2" s="13"/>
+      <c r="AE2" s="24"/>
     </row>
     <row r="3" spans="2:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="Y3" s="12" t="s">
+      <c r="Y3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AA3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AD3" s="12" t="s">
+      <c r="AD3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="12" t="s">
+      <c r="AE3" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.3">
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="AA4" s="12"/>
-      <c r="AB4" s="12"/>
-      <c r="AD4" s="12"/>
-      <c r="AE4" s="12"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -5453,11 +3428,11 @@
       <c r="N25" s="5">
         <v>0</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="16"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="18"/>
       <c r="U25" s="1">
         <f t="shared" si="0"/>
         <v>6.15</v>
@@ -5502,14 +3477,14 @@
       <c r="J26" s="5">
         <v>0</v>
       </c>
-      <c r="L26" s="14" t="s">
+      <c r="L26" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M26" s="15"/>
-      <c r="N26" s="16"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="19"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="21"/>
       <c r="U26" s="1">
         <f t="shared" si="0"/>
         <v>5.1000000000000005</v>
@@ -5546,9 +3521,9 @@
       <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="21"/>
       <c r="U27" s="1">
         <f t="shared" si="0"/>
         <v>5.25</v>
@@ -5567,24 +3542,24 @@
       </c>
     </row>
     <row r="28" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
-      <c r="H28" s="14" t="s">
+      <c r="E28" s="17"/>
+      <c r="F28" s="18"/>
+      <c r="H28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="16"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D29" s="17"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="19"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="4:31" x14ac:dyDescent="0.3">
       <c r="E30" s="8"/>
@@ -5596,126 +3571,126 @@
       <c r="F31" s="8"/>
     </row>
     <row r="34" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D34" s="23" t="s">
+      <c r="D34" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="H34" s="23" t="s">
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="H34" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="L34" s="23" t="s">
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="L34" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="P34" s="23" t="s">
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="P34" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
-      <c r="U34" s="13" t="s">
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="U34" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="V34" s="13"/>
-      <c r="X34" s="13" t="s">
+      <c r="V34" s="24"/>
+      <c r="X34" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="Y34" s="13"/>
-      <c r="AA34" s="13" t="s">
+      <c r="Y34" s="24"/>
+      <c r="AA34" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AB34" s="13"/>
-      <c r="AD34" s="13" t="s">
+      <c r="AB34" s="24"/>
+      <c r="AD34" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="AE34" s="13"/>
+      <c r="AE34" s="24"/>
     </row>
     <row r="35" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L35" s="21" t="s">
+      <c r="L35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M35" s="21" t="s">
+      <c r="M35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N35" s="21" t="s">
+      <c r="N35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="P35" s="21" t="s">
+      <c r="P35" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="Q35" s="21" t="s">
+      <c r="Q35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="R35" s="21" t="s">
+      <c r="R35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="U35" s="12" t="s">
+      <c r="U35" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="V35" s="12" t="s">
+      <c r="V35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="X35" s="12" t="s">
+      <c r="X35" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="Y35" s="12" t="s">
+      <c r="Y35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AA35" s="12" t="s">
+      <c r="AA35" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AB35" s="12" t="s">
+      <c r="AB35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="AD35" s="12" t="s">
+      <c r="AD35" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="AE35" s="12" t="s">
+      <c r="AE35" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-      <c r="P36" s="22"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="U36" s="12"/>
-      <c r="V36" s="12"/>
-      <c r="X36" s="12"/>
-      <c r="Y36" s="12"/>
-      <c r="AA36" s="12"/>
-      <c r="AB36" s="12"/>
-      <c r="AD36" s="12"/>
-      <c r="AE36" s="12"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
     </row>
     <row r="37" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D37" s="1">
@@ -7118,16 +5093,16 @@
       </c>
     </row>
     <row r="57" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="15"/>
-      <c r="F57" s="16"/>
-      <c r="H57" s="14" t="s">
+      <c r="E57" s="17"/>
+      <c r="F57" s="18"/>
+      <c r="H57" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I57" s="15"/>
-      <c r="J57" s="16"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="18"/>
       <c r="L57" s="1">
         <v>18.5</v>
       </c>
@@ -7164,12 +5139,12 @@
       </c>
     </row>
     <row r="58" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="17"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="19"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="18"/>
-      <c r="J58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="21"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="21"/>
       <c r="L58" s="9">
         <v>21</v>
       </c>
@@ -7206,30 +5181,30 @@
       </c>
     </row>
     <row r="59" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="L59" s="14" t="s">
+      <c r="L59" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="M59" s="15"/>
-      <c r="N59" s="16"/>
-      <c r="P59" s="14" t="s">
+      <c r="M59" s="17"/>
+      <c r="N59" s="18"/>
+      <c r="P59" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="16"/>
+      <c r="Q59" s="17"/>
+      <c r="R59" s="18"/>
     </row>
     <row r="60" spans="4:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L60" s="17"/>
-      <c r="M60" s="18"/>
-      <c r="N60" s="19"/>
-      <c r="P60" s="17"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="21"/>
+      <c r="P60" s="19"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="21"/>
     </row>
     <row r="63" spans="4:31" x14ac:dyDescent="0.3">
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="20"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="4:31" x14ac:dyDescent="0.3">
       <c r="D64" s="6">
@@ -7369,47 +5344,14 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="D28:F29"/>
-    <mergeCell ref="H28:J29"/>
-    <mergeCell ref="L26:N27"/>
-    <mergeCell ref="P25:R26"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="P35:P36"/>
-    <mergeCell ref="Q35:Q36"/>
-    <mergeCell ref="R35:R36"/>
-    <mergeCell ref="D57:F58"/>
-    <mergeCell ref="H57:J58"/>
-    <mergeCell ref="L59:N60"/>
-    <mergeCell ref="P59:R60"/>
-    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="AA35:AA36"/>
+    <mergeCell ref="AB35:AB36"/>
+    <mergeCell ref="AD35:AD36"/>
+    <mergeCell ref="AE35:AE36"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AD34:AE34"/>
     <mergeCell ref="V35:V36"/>
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="X3:X4"/>
@@ -7426,14 +5368,47 @@
     <mergeCell ref="X35:X36"/>
     <mergeCell ref="Y35:Y36"/>
     <mergeCell ref="AA34:AB34"/>
-    <mergeCell ref="AA35:AA36"/>
-    <mergeCell ref="AB35:AB36"/>
-    <mergeCell ref="AD35:AD36"/>
-    <mergeCell ref="AE35:AE36"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="D57:F58"/>
+    <mergeCell ref="H57:J58"/>
+    <mergeCell ref="L59:N60"/>
+    <mergeCell ref="P59:R60"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="P25:R26"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="P35:P36"/>
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="R35:R36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="D28:F29"/>
+    <mergeCell ref="H28:J29"/>
+    <mergeCell ref="L26:N27"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>